<commit_message>
Update dashboard (caixa fech)
</commit_message>
<xml_diff>
--- a/mapa_orientacao.xlsx
+++ b/mapa_orientacao.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estoque\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estoque\Documents\estoque.renan\projetos\projeto_curva_abc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F793504A-0689-4031-8991-B136BDEDB26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFECC08-44DF-4A40-BB7E-4AAA2FEF2AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{EAE29F3D-FD6F-4A84-9819-0A46C6FDAC5C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>10e12par</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>18par</t>
-  </si>
-  <si>
-    <t>CAP</t>
   </si>
 </sst>
 </file>
@@ -583,7 +580,7 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:N37"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1546,8 +1543,8 @@
       <c r="K22" s="4">
         <v>42</v>
       </c>
-      <c r="L22" s="4" t="s">
-        <v>14</v>
+      <c r="L22" s="4">
+        <v>41</v>
       </c>
       <c r="M22">
         <v>0</v>

</xml_diff>